<commit_message>
Backup before Live Share
</commit_message>
<xml_diff>
--- a/Edgewell US Male Dataset.xlsx
+++ b/Edgewell US Male Dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\Salma Hany\Documents\Slide-Automate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146C339B-A8C6-4F19-97B8-DD398BB0D6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B63616-44FA-48EE-9B94-F1F8A5F42297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="957" r:id="rId2"/>
+    <pivotCache cacheId="1072" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,9 +59,9 @@
     <s v="{[Products].[Category].&amp;[Manual Shave Men]}"/>
     <s v="{[Market].[Area].&amp;[RETAILER]}"/>
     <s v="{[Market].[Region].&amp;[Walmart]}"/>
+    <s v="{[Calendar].[MonthYear].&amp;[Apr-24],[Calendar].[MonthYear].&amp;[May-24],[Calendar].[MonthYear].&amp;[Jun-24],[Calendar].[MonthYear].&amp;[Jul-24],[Calendar].[MonthYear].&amp;[Aug-24],[Calendar].[MonthYear].&amp;[Sep-24],[Calendar].[MonthYear].&amp;[Oct-24],[Calendar].[MonthYear].&amp;[Nov-24],[Calendar].[MonthYear].&amp;[Dec-24],[Calendar].[MonthYear].&amp;[Jan-25],[Calendar].[MonthYear].&amp;[Feb-25],[Calendar].[MonthYear].&amp;[Mar-25]}"/>
     <s v="{[Scope].[Scope].&amp;[Segment]}"/>
-    <s v="{[Products].[Segment].&amp;[Disposables]}"/>
-    <s v="{[Calendar].[MonthYear].&amp;[Apr-24],[Calendar].[MonthYear].&amp;[May-24],[Calendar].[MonthYear].&amp;[Jun-24],[Calendar].[MonthYear].&amp;[Jul-24],[Calendar].[MonthYear].&amp;[Aug-24],[Calendar].[MonthYear].&amp;[Sep-24],[Calendar].[MonthYear].&amp;[Oct-24],[Calendar].[MonthYear].&amp;[Nov-24],[Calendar].[MonthYear].&amp;[Dec-24],[Calendar].[MonthYear].&amp;[Jan-25],[Calendar].[MonthYear].&amp;[Feb-25],[Calendar].[MonthYear].&amp;[Mar-25]}"/>
+    <s v="{[Products].[Sector].&amp;[Disposables]}"/>
   </metadataStrings>
   <mdxMetadata count="8">
     <mdx n="0" f="s">
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Scope</t>
   </si>
@@ -145,16 +145,7 @@
     <t>Market</t>
   </si>
   <si>
-    <t>MonthYear</t>
-  </si>
-  <si>
     <t>Brand</t>
-  </si>
-  <si>
-    <t>Segment</t>
-  </si>
-  <si>
-    <t>(Multiple Items)</t>
   </si>
   <si>
     <t>RETAILER</t>
@@ -163,16 +154,19 @@
     <t>Walmart</t>
   </si>
   <si>
-    <t>Disposables</t>
+    <t>Equate</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Values</t>
   </si>
   <si>
     <t>Barbasol</t>
   </si>
   <si>
     <t>Bic</t>
-  </si>
-  <si>
-    <t>Equate</t>
   </si>
   <si>
     <t>Gillette</t>
@@ -190,127 +184,61 @@
     <t>Wilkinson Sword</t>
   </si>
   <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Pack Size</t>
-  </si>
-  <si>
-    <t>1CT</t>
-  </si>
-  <si>
-    <t>2CT</t>
-  </si>
-  <si>
-    <t>5CT</t>
-  </si>
-  <si>
-    <t>10CT</t>
-  </si>
-  <si>
-    <t>3CT</t>
-  </si>
-  <si>
-    <t>4CT</t>
-  </si>
-  <si>
-    <t>6CT</t>
-  </si>
-  <si>
-    <t>15CT</t>
-  </si>
-  <si>
-    <t>Barbasol Total</t>
-  </si>
-  <si>
-    <t>8CT</t>
-  </si>
-  <si>
-    <t>20CT</t>
-  </si>
-  <si>
-    <t>7CT</t>
-  </si>
-  <si>
-    <t>9CT</t>
-  </si>
-  <si>
-    <t>12CT</t>
-  </si>
-  <si>
-    <t>18CT</t>
-  </si>
-  <si>
-    <t>21CT</t>
-  </si>
-  <si>
-    <t>24CT</t>
-  </si>
-  <si>
-    <t>52CT</t>
-  </si>
-  <si>
-    <t>Bic Total</t>
-  </si>
-  <si>
-    <t>Equate Total</t>
-  </si>
-  <si>
-    <t>25CT</t>
-  </si>
-  <si>
-    <t>Gillette Total</t>
-  </si>
-  <si>
-    <t>Harry's Total</t>
-  </si>
-  <si>
-    <t>Personna Total</t>
-  </si>
-  <si>
-    <t>Schick Total</t>
-  </si>
-  <si>
-    <t>Wilkinson Sword Total</t>
-  </si>
-  <si>
-    <t>SubCategory</t>
+    <t>MonthYear</t>
   </si>
   <si>
     <t>Av Price/Unit</t>
   </si>
   <si>
-    <t>Values</t>
-  </si>
-  <si>
     <t>Value Share</t>
   </si>
   <si>
-    <t>Sensitive Skin</t>
+    <t>(Multiple Items)</t>
   </si>
   <si>
-    <t>Normal Skin</t>
+    <t>Disposables</t>
   </si>
   <si>
-    <t>Rem Types</t>
+    <t>Segment</t>
   </si>
   <si>
-    <t>Sensitive Skin Total</t>
+    <t>Sector</t>
   </si>
   <si>
-    <t>Normal Skin Total</t>
+    <t>Disposables Total</t>
   </si>
   <si>
-    <t>Rem Types Total</t>
+    <t>Relative Price</t>
+  </si>
+  <si>
+    <t>Value Sales</t>
+  </si>
+  <si>
+    <t>IYA Price/KG</t>
+  </si>
+  <si>
+    <t>Base Price/KG</t>
+  </si>
+  <si>
+    <t>Av Price/KG</t>
+  </si>
+  <si>
+    <t>WoB %</t>
+  </si>
+  <si>
+    <t>Value Share DYA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="\$#,##0.00;\-\$#,##0.00;\$#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%;\-0.0%;0.0%"/>
+    <numFmt numFmtId="166" formatCode="#,##0%;\-#,##0%;#,##0%"/>
+    <numFmt numFmtId="167" formatCode="0%;\-0%;0%"/>
+    <numFmt numFmtId="168" formatCode="\+0.0%;\-0.0%;0.0%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -771,11 +699,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -835,9 +767,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Salma Hany" refreshedDate="45866.644905555557" backgroundQuery="1" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Salma Hany" refreshedDate="45875.559035995371" backgroundQuery="1" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="13">
+  <cacheFields count="19">
+    <cacheField name="[Products].[Segment].[Segment]" caption="Segment" numFmtId="0" hierarchy="103" level="1">
+      <sharedItems count="1">
+        <s v="[Products].[Segment].&amp;[Disposables]" c="Disposables"/>
+      </sharedItems>
+    </cacheField>
     <cacheField name="[Products].[Brand].[Brand]" caption="Brand" numFmtId="0" hierarchy="76" level="1">
       <sharedItems count="8">
         <s v="[Products].[Brand].&amp;[Barbasol]" c="Barbasol"/>
@@ -850,35 +787,6 @@
         <s v="[Products].[Brand].&amp;[Wilkinson Sword]" c="Wilkinson Sword"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Products].[SubCategory].[SubCategory]" caption="SubCategory" numFmtId="0" hierarchy="107" level="1">
-      <sharedItems count="3">
-        <s v="[Products].[SubCategory].&amp;[Normal Skin]" c="Normal Skin"/>
-        <s v="[Products].[SubCategory].&amp;[Sensitive Skin]" c="Sensitive Skin"/>
-        <s v="[Products].[SubCategory].&amp;[Rem Types]" c="Rem Types"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Products].[Pack Size].[Pack Size]" caption="Pack Size" numFmtId="0" hierarchy="93" level="1">
-      <sharedItems count="18">
-        <s v="[Products].[Pack Size].&amp;[3CT]" c="3CT"/>
-        <s v="[Products].[Pack Size].&amp;[4CT]" c="4CT"/>
-        <s v="[Products].[Pack Size].&amp;[1CT]" c="1CT"/>
-        <s v="[Products].[Pack Size].&amp;[2CT]" c="2CT"/>
-        <s v="[Products].[Pack Size].&amp;[6CT]" c="6CT"/>
-        <s v="[Products].[Pack Size].&amp;[8CT]" c="8CT"/>
-        <s v="[Products].[Pack Size].&amp;[10CT]" c="10CT"/>
-        <s v="[Products].[Pack Size].&amp;[12CT]" c="12CT"/>
-        <s v="[Products].[Pack Size].&amp;[18CT]" c="18CT"/>
-        <s v="[Products].[Pack Size].&amp;[5CT]" c="5CT"/>
-        <s v="[Products].[Pack Size].&amp;[7CT]" c="7CT"/>
-        <s v="[Products].[Pack Size].&amp;[24CT]" c="24CT"/>
-        <s v="[Products].[Pack Size].&amp;[52CT]" c="52CT"/>
-        <s v="[Products].[Pack Size].&amp;[15CT]" c="15CT"/>
-        <s v="[Products].[Pack Size].&amp;[21CT]" c="21CT"/>
-        <s v="[Products].[Pack Size].&amp;[25CT]" c="25CT"/>
-        <s v="[Products].[Pack Size].&amp;[9CT]" c="9CT"/>
-        <s v="[Products].[Pack Size].&amp;[20CT]" c="20CT"/>
-      </sharedItems>
-    </cacheField>
     <cacheField name="[Products].[Category].[Category]" caption="Category" numFmtId="0" hierarchy="81" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
@@ -886,6 +794,9 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
     <cacheField name="[Calendar].[MonthYear].[MonthYear]" caption="MonthYear" numFmtId="0" hierarchy="35" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Products].[Sector].[Sector]" caption="Sector" numFmtId="0" hierarchy="102" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
     <cacheField name="[Market].[Area].[Area]" caption="Area" numFmtId="0" hierarchy="58" level="1">
@@ -900,11 +811,15 @@
     <cacheField name="[Market].[Market].[Market]" caption="Market" numFmtId="0" hierarchy="63" level="1">
       <sharedItems containsSemiMixedTypes="0" containsString="0"/>
     </cacheField>
-    <cacheField name="[Products].[Segment].[Segment]" caption="Segment" numFmtId="0" hierarchy="103" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
+    <cacheField name="[Measures].[Relative Price]" caption="Relative Price" numFmtId="0" hierarchy="564" level="32767"/>
     <cacheField name="[Measures].[Av Price/Unit]" caption="Av Price/Unit" numFmtId="0" hierarchy="549" level="32767"/>
+    <cacheField name="[Measures].[Value Sales]" caption="Value Sales" numFmtId="0" hierarchy="448" level="32767"/>
+    <cacheField name="[Measures].[IYA Price/KG]" caption="IYA Price/KG" numFmtId="0" hierarchy="559" level="32767"/>
+    <cacheField name="[Measures].[Base Price/KG]" caption="Base Price/KG" numFmtId="0" hierarchy="689" level="32767"/>
+    <cacheField name="[Measures].[Av Price/KG]" caption="Av Price/KG" numFmtId="0" hierarchy="550" level="32767"/>
     <cacheField name="[Measures].[Value Share]" caption="Value Share" numFmtId="0" hierarchy="639" level="32767"/>
+    <cacheField name="[Measures].[WoB %]" caption="WoB %" numFmtId="0" hierarchy="1366" level="32767"/>
+    <cacheField name="[Measures].[Value Share DYA]" caption="Value Share DYA" numFmtId="0" hierarchy="648" level="32767"/>
   </cacheFields>
   <cacheHierarchies count="2657">
     <cacheHierarchy uniqueName="[2nd Measure Table].[Measures]" caption="Measures" attribute="1" defaultMemberUniqueName="[2nd Measure Table].[Measures].[All]" allUniqueName="[2nd Measure Table].[Measures].[All]" dimensionUniqueName="[2nd Measure Table]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
@@ -945,7 +860,7 @@
     <cacheHierarchy uniqueName="[Calendar].[MonthYear]" caption="MonthYear" attribute="1" time="1" defaultMemberUniqueName="[Calendar].[MonthYear].[All]" allUniqueName="[Calendar].[MonthYear].[All]" dimensionUniqueName="[Calendar]" displayFolder="Month" count="2" memberValueDatatype="130" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="5"/>
+        <fieldUsage x="4"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Calendar].[MonthYearLong]" caption="MonthYearLong" attribute="1" time="1" defaultMemberUniqueName="[Calendar].[MonthYearLong].[All]" allUniqueName="[Calendar].[MonthYearLong].[All]" dimensionUniqueName="[Calendar]" displayFolder="Month" count="0" memberValueDatatype="130" unbalanced="0"/>
@@ -1011,7 +926,7 @@
     <cacheHierarchy uniqueName="[Products].[Brand]" caption="Brand" attribute="1" defaultMemberUniqueName="[Products].[Brand].[All]" allUniqueName="[Products].[Brand].[All]" dimensionUniqueName="[Products]" displayFolder="Company &amp; Product" count="2" memberValueDatatype="130" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="0"/>
+        <fieldUsage x="1"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Products].[Brand Logo URL]" caption="Brand Logo URL" attribute="1" defaultMemberUniqueName="[Products].[Brand Logo URL].[All]" allUniqueName="[Products].[Brand Logo URL].[All]" dimensionUniqueName="[Products]" displayFolder="Images" count="0" memberValueDatatype="130" unbalanced="0"/>
@@ -1021,7 +936,7 @@
     <cacheHierarchy uniqueName="[Products].[Category]" caption="Category" attribute="1" defaultMemberUniqueName="[Products].[Category].[All]" allUniqueName="[Products].[Category].[All]" dimensionUniqueName="[Products]" displayFolder="Category" count="2" memberValueDatatype="130" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="3"/>
+        <fieldUsage x="2"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Products].[Category Hierarchy]" caption="Category Hierarchy" defaultMemberUniqueName="[Products].[Category Hierarchy].[All]" allUniqueName="[Products].[Category Hierarchy].[All]" dimensionUniqueName="[Products]" displayFolder="" count="6" unbalanced="0"/>
@@ -1035,12 +950,7 @@
     <cacheHierarchy uniqueName="[Products].[MANUFACTURER Hierarchy]" caption="MANUFACTURER Hierarchy" defaultMemberUniqueName="[Products].[MANUFACTURER Hierarchy].[All]" allUniqueName="[Products].[MANUFACTURER Hierarchy].[All]" dimensionUniqueName="[Products]" displayFolder="" count="9" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Pack Count]" caption="Pack Count" attribute="1" defaultMemberUniqueName="[Products].[Pack Count].[All]" allUniqueName="[Products].[Pack Count].[All]" dimensionUniqueName="[Products]" displayFolder="Pack Size" count="0" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Pack Count Bracket]" caption="Pack Count Bracket" attribute="1" defaultMemberUniqueName="[Products].[Pack Count Bracket].[All]" allUniqueName="[Products].[Pack Count Bracket].[All]" dimensionUniqueName="[Products]" displayFolder="Brackets" count="0" memberValueDatatype="130" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Products].[Pack Size]" caption="Pack Size" attribute="1" defaultMemberUniqueName="[Products].[Pack Size].[All]" allUniqueName="[Products].[Pack Size].[All]" dimensionUniqueName="[Products]" displayFolder="Pack Size" count="2" memberValueDatatype="130" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Products].[Pack Size]" caption="Pack Size" attribute="1" defaultMemberUniqueName="[Products].[Pack Size].[All]" allUniqueName="[Products].[Pack Size].[All]" dimensionUniqueName="[Products]" displayFolder="Pack Size" count="2" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Pack Size Bracket]" caption="Pack Size Bracket" attribute="1" defaultMemberUniqueName="[Products].[Pack Size Bracket].[All]" allUniqueName="[Products].[Pack Size Bracket].[All]" dimensionUniqueName="[Products]" displayFolder="Brackets" count="0" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Pack Type]" caption="Pack Type" attribute="1" defaultMemberUniqueName="[Products].[Pack Type].[All]" allUniqueName="[Products].[Pack Type].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[PackConfiguration]" caption="PackConfiguration" attribute="1" defaultMemberUniqueName="[Products].[PackConfiguration].[All]" allUniqueName="[Products].[PackConfiguration].[All]" dimensionUniqueName="[Products]" displayFolder="Pack Size" count="0" memberValueDatatype="130" unbalanced="0"/>
@@ -1049,22 +959,22 @@
     <cacheHierarchy uniqueName="[Products].[Portion Size]" caption="Portion Size" attribute="1" defaultMemberUniqueName="[Products].[Portion Size].[All]" allUniqueName="[Products].[Portion Size].[All]" dimensionUniqueName="[Products]" displayFolder="Pack Size" count="0" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Portion Size Bracket]" caption="Portion Size Bracket" attribute="1" defaultMemberUniqueName="[Products].[Portion Size Bracket].[All]" allUniqueName="[Products].[Portion Size Bracket].[All]" dimensionUniqueName="[Products]" displayFolder="Brackets" count="0" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Product]" caption="Product" attribute="1" defaultMemberUniqueName="[Products].[Product].[All]" allUniqueName="[Products].[Product].[All]" dimensionUniqueName="[Products]" displayFolder="Company &amp; Product" count="2" memberValueDatatype="130" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Products].[Sector]" caption="Sector" attribute="1" defaultMemberUniqueName="[Products].[Sector].[All]" allUniqueName="[Products].[Sector].[All]" dimensionUniqueName="[Products]" displayFolder="Category" count="2" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Products].[Sector]" caption="Sector" attribute="1" defaultMemberUniqueName="[Products].[Sector].[All]" allUniqueName="[Products].[Sector].[All]" dimensionUniqueName="[Products]" displayFolder="Category" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="5"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Products].[Segment]" caption="Segment" attribute="1" defaultMemberUniqueName="[Products].[Segment].[All]" allUniqueName="[Products].[Segment].[All]" dimensionUniqueName="[Products]" displayFolder="Category" count="2" memberValueDatatype="130" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="10"/>
+        <fieldUsage x="0"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Products].[SKU]" caption="SKU" attribute="1" defaultMemberUniqueName="[Products].[SKU].[All]" allUniqueName="[Products].[SKU].[All]" dimensionUniqueName="[Products]" displayFolder="Company &amp; Product" count="2" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Store Link]" caption="Store Link" attribute="1" defaultMemberUniqueName="[Products].[Store Link].[All]" allUniqueName="[Products].[Store Link].[All]" dimensionUniqueName="[Products]" displayFolder="Images" count="0" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[SubBrand]" caption="SubBrand" attribute="1" defaultMemberUniqueName="[Products].[SubBrand].[All]" allUniqueName="[Products].[SubBrand].[All]" dimensionUniqueName="[Products]" displayFolder="Company &amp; Product" count="2" memberValueDatatype="130" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Products].[SubCategory]" caption="SubCategory" attribute="1" defaultMemberUniqueName="[Products].[SubCategory].[All]" allUniqueName="[Products].[SubCategory].[All]" dimensionUniqueName="[Products]" displayFolder="Category" count="2" memberValueDatatype="130" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Products].[SubCategory]" caption="SubCategory" attribute="1" defaultMemberUniqueName="[Products].[SubCategory].[All]" allUniqueName="[Products].[SubCategory].[All]" dimensionUniqueName="[Products]" displayFolder="Category" count="2" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[SubSegment]" caption="SubSegment" attribute="1" defaultMemberUniqueName="[Products].[SubSegment].[All]" allUniqueName="[Products].[SubSegment].[All]" dimensionUniqueName="[Products]" displayFolder="Category" count="2" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Top Brands]" caption="Top Brands" attribute="1" defaultMemberUniqueName="[Products].[Top Brands].[All]" allUniqueName="[Products].[Top Brands].[All]" dimensionUniqueName="[Products]" displayFolder="Company &amp; Product" count="2" memberValueDatatype="130" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Top Companies]" caption="Top Companies" attribute="1" defaultMemberUniqueName="[Products].[Top Companies].[All]" allUniqueName="[Products].[Top Companies].[All]" dimensionUniqueName="[Products]" displayFolder="Company &amp; Product" count="2" memberValueDatatype="130" unbalanced="0"/>
@@ -1105,7 +1015,7 @@
     <cacheHierarchy uniqueName="[Scope].[Scope]" caption="Scope" attribute="1" defaultMemberUniqueName="[Scope].[Scope].[All]" allUniqueName="[Scope].[Scope].[All]" dimensionUniqueName="[Scope]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="4"/>
+        <fieldUsage x="3"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Shelf Price Ladder].[Shelf Price Group]" caption="Shelf Price Group" attribute="1" defaultMemberUniqueName="[Shelf Price Ladder].[Shelf Price Group].[All]" allUniqueName="[Shelf Price Ladder].[Shelf Price Group].[All]" dimensionUniqueName="[Shelf Price Ladder]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
@@ -1410,7 +1320,11 @@
     <cacheHierarchy uniqueName="[VAT].[VAT SORT]" caption="VAT SORT" attribute="1" defaultMemberUniqueName="[VAT].[VAT SORT].[All]" allUniqueName="[VAT].[VAT SORT].[All]" dimensionUniqueName="[VAT]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0" hidden="1"/>
     <cacheHierarchy uniqueName="[Measures].[Unit Sales]" caption="Unit Sales" measure="1" displayFolder="Unit Sales" measureGroup="Sales Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Volume Sales]" caption="Volume Sales" measure="1" displayFolder="Volume Sales" measureGroup="Sales Metrics" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Value Sales]" caption="Value Sales" measure="1" displayFolder="Value Sales" measureGroup="Sales Metrics" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Value Sales]" caption="Value Sales" measure="1" displayFolder="Value Sales" measureGroup="Sales Metrics" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="12"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Unit Sales PP]" caption="Unit Sales PP" measure="1" displayFolder="Unit Sales" measureGroup="Sales Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Unit Sales YA]" caption="Unit Sales YA" measure="1" displayFolder="Unit Sales" measureGroup="Sales Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Volume Sales PP]" caption="Volume Sales PP" measure="1" displayFolder="Volume Sales" measureGroup="Sales Metrics" count="0"/>
@@ -1516,7 +1430,11 @@
         <fieldUsage x="11"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Av Price/KG]" caption="Av Price/KG" measure="1" displayFolder="Price/KG" measureGroup="Price Metrics" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Av Price/KG]" caption="Av Price/KG" measure="1" displayFolder="Price/KG" measureGroup="Price Metrics" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="15"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[YA Price/Unit]" caption="YA Price/Unit" measure="1" displayFolder="Price/Unit" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[YA Price/KG]" caption="YA Price/KG" measure="1" displayFolder="Price/KG" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[PP Price/KG]" caption="PP Price/KG" measure="1" displayFolder="Price/KG" measureGroup="Price Metrics" count="0"/>
@@ -1525,12 +1443,20 @@
     <cacheHierarchy uniqueName="[Measures].[DPP Price/Unit]" caption="DPP Price/Unit" measure="1" displayFolder="Price/Unit" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[DYA Price/KG]" caption="DYA Price/KG" measure="1" displayFolder="Price/KG" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[DYA Price/Unit]" caption="DYA Price/Unit" measure="1" displayFolder="Price/Unit" measureGroup="Price Metrics" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[IYA Price/KG]" caption="IYA Price/KG" measure="1" displayFolder="Price/KG" measureGroup="Price Metrics" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[IYA Price/KG]" caption="IYA Price/KG" measure="1" displayFolder="Price/KG" measureGroup="Price Metrics" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="13"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[IYA Price/Unit]" caption="IYA Price/Unit" measure="1" displayFolder="Price/Unit" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[IPP Price/KG]" caption="IPP Price/KG" measure="1" displayFolder="Price/KG" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[IPP Price/Unit]" caption="IPP Price/Unit" measure="1" displayFolder="Price/Unit" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Relative Price Index]" caption="Relative Price Index" measure="1" displayFolder="Relative Price" measureGroup="Price Metrics" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Relative Price]" caption="Relative Price" measure="1" displayFolder="Relative Price" measureGroup="Price Metrics" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Relative Price]" caption="Relative Price" measure="1" displayFolder="Relative Price" measureGroup="Price Metrics" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="10"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Channel Relative Price]" caption="Channel Relative Price" measure="1" displayFolder="Relative Price" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Price]" caption="Price" measure="1" displayFolder="" measureGroup="Price Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Price Evolution]" caption="Price Evolution" measure="1" displayFolder="" measureGroup="Price Metrics" count="0"/>
@@ -1607,7 +1533,7 @@
     <cacheHierarchy uniqueName="[Measures].[Company Sales]" caption="Company Sales" measure="1" displayFolder="" measureGroup="Market Sales" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Value Share]" caption="Value Share" measure="1" displayFolder="Value Share" measureGroup="Share Metrics" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="12"/>
+        <fieldUsage x="16"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Volume Share]" caption="Volume Share" measure="1" displayFolder="Volume Share" measureGroup="Share Metrics" count="0"/>
@@ -1618,7 +1544,11 @@
     <cacheHierarchy uniqueName="[Measures].[Unit Share PP]" caption="Unit Share PP" measure="1" displayFolder="Unit Share" measureGroup="Share Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Volume Share YA]" caption="Volume Share YA" measure="1" displayFolder="Volume Share" measureGroup="Share Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Volume Share PP]" caption="Volume Share PP" measure="1" displayFolder="Volume Share" measureGroup="Share Metrics" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Value Share DYA]" caption="Value Share DYA" measure="1" displayFolder="Value Share" measureGroup="Share Metrics" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Value Share DYA]" caption="Value Share DYA" measure="1" displayFolder="Value Share" measureGroup="Share Metrics" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="18"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Value Share DPP]" caption="Value Share DPP" measure="1" displayFolder="Value Share" measureGroup="Share Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Volume Share DYA]" caption="Volume Share DYA" measure="1" displayFolder="Volume Share" measureGroup="Share Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Volume Share DPP]" caption="Volume Share DPP" measure="1" displayFolder="Volume Share" measureGroup="Share Metrics" count="0"/>
@@ -1659,7 +1589,11 @@
     <cacheHierarchy uniqueName="[Measures].[Value Uplift (v. base)]" caption="Value Uplift (v. base)" measure="1" displayFolder="Uplift" measureGroup="Promo Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Units Uplift (v. Base)]" caption="Units Uplift (v. Base)" measure="1" displayFolder="Uplift" measureGroup="Promo Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[VSOD]" caption="VSOD" measure="1" displayFolder="KPIs" measureGroup="Promo Metrics" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Base Price/KG]" caption="Base Price/KG" measure="1" displayFolder="Base\Base Price" measureGroup="Promo Metrics" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Base Price/KG]" caption="Base Price/KG" measure="1" displayFolder="Base\Base Price" measureGroup="Promo Metrics" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="14"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Promo Price/KG]" caption="Promo Price/KG" measure="1" displayFolder="Promo Price" measureGroup="Promo Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Base Price/Unit]" caption="Base Price/Unit" measure="1" displayFolder="Base\Base Price" measureGroup="Promo Metrics" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Promo Price/Unit]" caption="Promo Price/Unit" measure="1" displayFolder="Promo Price" measureGroup="Promo Metrics" count="0"/>
@@ -2336,7 +2270,11 @@
     <cacheHierarchy uniqueName="[Measures].[Trade WoB %]" caption="Trade WoB %" measure="1" displayFolder="WoB" measureGroup="Distribution" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Area Weight DYA]" caption="Area Weight DYA" measure="1" displayFolder="WoB" measureGroup="Distribution" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Price Bracket WoB %]" caption="Price Bracket WoB %" measure="1" displayFolder="WoB" measureGroup="Distribution" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[WoB %]" caption="WoB %" measure="1" displayFolder="WoB" measureGroup="Distribution" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[WoB %]" caption="WoB %" measure="1" displayFolder="WoB" measureGroup="Distribution" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="17"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[ND PP]" caption="ND PP" measure="1" displayFolder="Numeric" measureGroup="Distribution" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[ND YA]" caption="ND YA" measure="1" displayFolder="Numeric" measureGroup="Distribution" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[ND DYA]" caption="ND DYA" measure="1" displayFolder="Numeric" measureGroup="Distribution" count="0"/>
@@ -3791,9 +3729,15 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="957" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="A16:E109" firstHeaderRow="1" firstDataRow="2" firstDataCol="3" rowPageCount="8" colPageCount="1"/>
-  <pivotFields count="13">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1072" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A16:K27" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="8" colPageCount="1"/>
+  <pivotFields count="19">
+    <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="9">
         <item x="0"/>
@@ -3804,37 +3748,6 @@
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" compact="0" allDrilled="1" outline="0" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
-      <items count="19">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3880,307 +3793,46 @@
     </pivotField>
     <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
     <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
   </pivotFields>
-  <rowFields count="3">
+  <rowFields count="2">
     <field x="0"/>
     <field x="1"/>
-    <field x="2"/>
   </rowFields>
-  <rowItems count="92">
+  <rowItems count="10">
     <i>
       <x/>
-      <x/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="4"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
-    <i r="2">
-      <x v="7"/>
-    </i>
-    <i r="2">
-      <x v="8"/>
-    </i>
-    <i t="default" r="1">
       <x/>
     </i>
     <i r="1">
       <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="4"/>
-    </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
-    <i r="2">
-      <x v="7"/>
-    </i>
-    <i r="2">
-      <x v="11"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="7"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x/>
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="9"/>
-    </i>
-    <i r="2">
-      <x v="4"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
-    <i r="2">
-      <x v="7"/>
-    </i>
-    <i r="2">
-      <x v="13"/>
-    </i>
-    <i r="2">
-      <x v="8"/>
-    </i>
-    <i r="2">
-      <x v="14"/>
-    </i>
-    <i r="2">
-      <x v="15"/>
-    </i>
-    <i r="2">
-      <x v="12"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
     </i>
     <i r="1">
       <x v="2"/>
-      <x v="16"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
     </i>
     <i r="1">
-      <x v="1"/>
-      <x v="2"/>
+      <x v="3"/>
     </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
+    <i r="1">
       <x v="4"/>
     </i>
-    <i r="2">
-      <x v="10"/>
-    </i>
-    <i r="2">
+    <i r="1">
       <x v="5"/>
     </i>
-    <i r="2">
+    <i r="1">
       <x v="6"/>
     </i>
-    <i r="2">
+    <i r="1">
       <x v="7"/>
     </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
     <i t="default">
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
       <x/>
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i t="default">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x/>
-      <x v="6"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i t="default">
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-      <x/>
-      <x v="3"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
-    <i r="2">
-      <x v="7"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-      <x v="5"/>
-    </i>
-    <i t="default" r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-      <x v="2"/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x v="4"/>
-    </i>
-    <i r="2">
-      <x v="5"/>
-    </i>
-    <i r="2">
-      <x v="6"/>
-    </i>
-    <i r="2">
-      <x v="7"/>
-    </i>
-    <i r="2">
-      <x v="17"/>
-    </i>
-    <i t="default" r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x/>
-      <x v="5"/>
-    </i>
-    <i t="default" r="1">
-      <x/>
-    </i>
-    <i t="default">
-      <x v="7"/>
     </i>
     <i t="grand">
       <x/>
@@ -4189,27 +3841,55 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="9">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+    <i i="6">
+      <x v="6"/>
+    </i>
+    <i i="7">
+      <x v="7"/>
+    </i>
+    <i i="8">
+      <x v="8"/>
+    </i>
   </colItems>
   <pageFields count="8">
-    <pageField fld="3" hier="81" name="[Products].[Category].&amp;[Manual Shave Men]" cap="Manual Shave Men"/>
-    <pageField fld="4" hier="145" name="[Scope].[Scope].&amp;[Segment]" cap="Segment"/>
-    <pageField fld="5" hier="35" name="[Calendar].[MonthYear].[All]" cap="All"/>
+    <pageField fld="2" hier="81" name="[Products].[Category].&amp;[Manual Shave Men]" cap="Manual Shave Men"/>
+    <pageField fld="3" hier="145" name="[Scope].[Scope].&amp;[Segment]" cap="Segment"/>
+    <pageField fld="4" hier="35" name="[Calendar].[MonthYear].[All]" cap="All"/>
+    <pageField fld="5" hier="102" name="[Products].[Sector].&amp;[Disposables]" cap="Disposables"/>
     <pageField fld="6" hier="58" name="[Market].[Area].&amp;[RETAILER]" cap="RETAILER"/>
     <pageField fld="7" hier="64" name="[Market].[Region].&amp;[Walmart]" cap="Walmart"/>
     <pageField fld="8" hier="59" name="[Market].[Channel].[All]" cap="All"/>
     <pageField fld="9" hier="63" name="[Market].[Market].[All]" cap="All"/>
-    <pageField fld="10" hier="103" name="[Products].[Segment].&amp;[Disposables]" cap="Disposables"/>
   </pageFields>
-  <dataFields count="2">
+  <dataFields count="9">
+    <dataField fld="10" baseField="0" baseItem="0"/>
     <dataField fld="11" baseField="0" baseItem="0"/>
     <dataField fld="12" baseField="0" baseItem="0"/>
+    <dataField fld="13" baseField="0" baseItem="0"/>
+    <dataField fld="14" baseField="0" baseItem="0"/>
+    <dataField fld="15" baseField="0" baseItem="0"/>
+    <dataField fld="16" baseField="0" baseItem="0"/>
+    <dataField fld="17" baseField="0" baseItem="0"/>
+    <dataField fld="18" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotHierarchies count="2657">
     <pivotHierarchy/>
@@ -6886,10 +6566,9 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleMedium21" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="3">
+  <rowHierarchiesUsage count="2">
+    <rowHierarchyUsage hierarchyUsage="103"/>
     <rowHierarchyUsage hierarchyUsage="76"/>
-    <rowHierarchyUsage hierarchyUsage="107"/>
-    <rowHierarchyUsage hierarchyUsage="93"/>
   </rowHierarchiesUsage>
   <colHierarchiesUsage count="1">
     <colHierarchyUsage hierarchyUsage="-2"/>
@@ -7199,25 +6878,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A7:E109"/>
+  <dimension ref="A7:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C14005" sqref="C14005"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
@@ -7236,7 +6914,7 @@
     <col min="103" max="103" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -7244,1159 +6922,420 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s" vm="6">
+      <c r="B8" t="s" vm="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" vm="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s" vm="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s" vm="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s" vm="5">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s" vm="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s" vm="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s" vm="8">
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1.58</v>
+      </c>
+      <c r="D18" s="2">
         <v>11</v>
       </c>
+      <c r="E18" s="5">
+        <v>22</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1.179</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.8332999999999999</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.4666999999999999</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1.3598818030297006E-7</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
+        <v>-4.8347746888349138E-7</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s" vm="4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5.2460000000000004</v>
+      </c>
+      <c r="E19" s="5">
+        <v>29854336</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.77959999999999996</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.78159999999999996</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.18453803758152043</v>
+      </c>
+      <c r="J19" s="6">
+        <v>0.1845</v>
+      </c>
+      <c r="K19" s="7">
+        <v>6.3656479803893828E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3.3515999999999999</v>
+      </c>
+      <c r="E20" s="5">
+        <v>24797807</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.54910000000000003</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.54459999999999997</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.15328221133792058</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0.15329999999999999</v>
+      </c>
+      <c r="K20" s="7">
+        <v>7.0539345932639219E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="D21" s="2">
+        <v>10.2652</v>
+      </c>
+      <c r="E21" s="5">
+        <v>87493817</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.2384999999999999</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1.2369000000000001</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.54082386189050302</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0.54079999999999995</v>
+      </c>
+      <c r="K21" s="7">
+        <v>4.3554912445610272E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1.302</v>
+      </c>
+      <c r="D22" s="2">
+        <v>6.7435999999999998</v>
+      </c>
+      <c r="E22" s="5">
+        <v>529274</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1.109</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.2119</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1.2088000000000001</v>
+      </c>
+      <c r="I22" s="3">
+        <v>3.2715912791670076E-3</v>
+      </c>
+      <c r="J22" s="6">
+        <v>3.3E-3</v>
+      </c>
+      <c r="K22" s="7">
+        <v>-1.1246129040241231E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.251</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2.3332999999999999</v>
+      </c>
+      <c r="E23" s="5">
+        <v>7</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1.8660000000000001</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.23330000000000001</v>
+      </c>
+      <c r="I23" s="3">
+        <v>4.3268966460035926E-8</v>
+      </c>
+      <c r="J23" s="6">
+        <v>0</v>
+      </c>
+      <c r="K23" s="7">
+        <v>1.7723991235851948E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>8.3892000000000007</v>
+      </c>
+      <c r="E24" s="5">
+        <v>19103492</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.98709999999999998</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.98740000000000006</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.11808405065965208</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0.1181</v>
+      </c>
+      <c r="K24" s="7">
+        <v>-6.5284831561474993E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.37</v>
+      </c>
+      <c r="D25" s="2">
+        <v>3.6667000000000001</v>
+      </c>
+      <c r="E25" s="5">
+        <v>11</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.34379999999999999</v>
+      </c>
+      <c r="I25" s="3">
+        <v>6.7994090151485029E-8</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0</v>
+      </c>
+      <c r="K25" s="7">
+        <v>4.1316520910250806E-9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6.7496</v>
+      </c>
+      <c r="E26" s="5">
+        <v>161778766</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.93069999999999997</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.9284</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s" vm="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s" vm="1">
+      <c r="C27" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s" vm="2">
+      <c r="D27" s="2">
+        <v>6.7496</v>
+      </c>
+      <c r="E27" s="5">
+        <v>161778766</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.93069999999999997</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.9284</v>
+      </c>
+      <c r="I27" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s" vm="7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D16" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="2">
-        <v>9</v>
-      </c>
-      <c r="E18" s="3">
-        <v>5.5631528305760471E-8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="2">
-        <v>13</v>
-      </c>
-      <c r="E19" s="3">
-        <v>8.0356651997209573E-8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="2">
-        <v>11</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1.3598818030297006E-7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="2">
-        <v>11</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1.3598818030297006E-7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1.9098999999999999</v>
-      </c>
-      <c r="E22" s="3">
-        <v>2.8817131662383926E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5.9901</v>
-      </c>
-      <c r="E23" s="3">
-        <v>3.651074331967645E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="2">
-        <v>10.915699999999999</v>
-      </c>
-      <c r="E24" s="3">
-        <v>2.221899133536474E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="2">
-        <v>9.5553000000000008</v>
-      </c>
-      <c r="E25" s="3">
-        <v>4.4063940999525238E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="2">
-        <v>4.9801000000000002</v>
-      </c>
-      <c r="E26" s="3">
-        <v>3.2828535730084628E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="2">
-        <v>5.8822000000000001</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1.6323359766509778E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="2">
-        <v>10</v>
-      </c>
-      <c r="E28" s="3">
-        <v>6.181280922862275E-8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5</v>
-      </c>
-      <c r="E29" s="3">
-        <v>3.0906404614311375E-8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="2">
-        <v>6.8739999999999997</v>
-      </c>
-      <c r="E30" s="3">
-        <v>8.2771251945388188E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1.0832999999999999</v>
-      </c>
-      <c r="E31" s="3">
-        <v>1.6071330399441915E-7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="2">
-        <v>6.9260999999999999</v>
-      </c>
-      <c r="E32" s="3">
-        <v>2.7693745667462934E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="2">
-        <v>6.4462000000000002</v>
-      </c>
-      <c r="E33" s="3">
-        <v>2.0445847633675237E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="2">
-        <v>3.9830999999999999</v>
-      </c>
-      <c r="E34" s="3">
-        <v>2.0366739600424448E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="2">
-        <v>4.9180999999999999</v>
-      </c>
-      <c r="E35" s="3">
-        <v>1.1855702991330767E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="2">
-        <v>4</v>
-      </c>
-      <c r="E36" s="3">
-        <v>2.4725123691449099E-8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="2">
-        <v>12.9671</v>
-      </c>
-      <c r="E37" s="3">
-        <v>2.3216334830987646E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="2">
-        <v>5.4809999999999999</v>
-      </c>
-      <c r="E38" s="3">
-        <v>8.8225237173585568E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="E39" s="3">
-        <v>1.2980689938010778E-7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" s="2">
-        <v>3.4321999999999999</v>
-      </c>
-      <c r="E40" s="3">
-        <v>3.5184376421810513E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="2">
-        <v>2</v>
-      </c>
-      <c r="E41" s="3">
-        <v>1.236256184572455E-8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="2">
-        <v>8.4</v>
-      </c>
-      <c r="E42" s="3">
-        <v>2.5961379876021556E-7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>58</v>
-      </c>
-      <c r="D43" s="2">
-        <v>4.3986999999999998</v>
-      </c>
-      <c r="E43" s="3">
-        <v>0.10176678563613224</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" s="2">
-        <v>5.2460000000000004</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0.18453803758152043</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="2">
-        <v>1.9370000000000001</v>
-      </c>
-      <c r="E45" s="3">
-        <v>2.0521852663902753E-5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
-        <v>29</v>
-      </c>
-      <c r="D46" s="2">
-        <v>5.0484</v>
-      </c>
-      <c r="E46" s="3">
-        <v>7.421648277376526E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="2">
-        <v>1.0034000000000001</v>
-      </c>
-      <c r="E47" s="3">
-        <v>1.0835352768112967E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" s="2">
-        <v>2.1772999999999998</v>
-      </c>
-      <c r="E48" s="3">
-        <v>2.3807982315800332E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>59</v>
-      </c>
-      <c r="D49" s="2">
-        <v>2.9874999999999998</v>
-      </c>
-      <c r="E49" s="3">
-        <v>0.10888033971034246</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="E50" s="3">
-        <v>1.6689458491728143E-7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="2">
-        <v>3.972</v>
-      </c>
-      <c r="E51" s="3">
-        <v>2.2045915469524599E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" s="2">
-        <v>5.9797000000000002</v>
-      </c>
-      <c r="E52" s="3">
-        <v>2.2355789263468605E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
-        <v>58</v>
-      </c>
-      <c r="D53" s="2">
-        <v>4.78</v>
-      </c>
-      <c r="E53" s="3">
-        <v>4.4401871627578124E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>44</v>
-      </c>
-      <c r="D54" s="2">
-        <v>3.3515999999999999</v>
-      </c>
-      <c r="E54" s="3">
-        <v>0.15328221133792058</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" t="s">
-        <v>26</v>
-      </c>
-      <c r="D55" s="2">
-        <v>9.9791000000000007</v>
-      </c>
-      <c r="E55" s="3">
-        <v>2.3011759157564596E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>29</v>
-      </c>
-      <c r="D56" s="2">
-        <v>6.9650999999999996</v>
-      </c>
-      <c r="E56" s="3">
-        <v>3.5912345876096E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>30</v>
-      </c>
-      <c r="D57" s="2">
-        <v>6.9947999999999997</v>
-      </c>
-      <c r="E57" s="3">
-        <v>2.3255017287002917E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" s="2">
-        <v>3.5127999999999999</v>
-      </c>
-      <c r="E58" s="3">
-        <v>5.0810129185927899E-6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
-        <v>31</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="3">
-        <v>4.3268966460035926E-8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="2">
-        <v>12.014200000000001</v>
-      </c>
-      <c r="E60" s="3">
-        <v>1.6019314920476029E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
-        <v>28</v>
-      </c>
-      <c r="D61" s="2">
-        <v>9.9687000000000001</v>
-      </c>
-      <c r="E61" s="3">
-        <v>5.2849914802786911E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
-        <v>38</v>
-      </c>
-      <c r="D62" s="2">
-        <v>10.818899999999999</v>
-      </c>
-      <c r="E62" s="3">
-        <v>9.0276501429118333E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" s="2">
-        <v>15.0128</v>
-      </c>
-      <c r="E63" s="3">
-        <v>2.2180574674429153E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
-        <v>39</v>
-      </c>
-      <c r="D64" s="2">
-        <v>14.9922</v>
-      </c>
-      <c r="E64" s="3">
-        <v>4.3111387065469395E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" s="2">
-        <v>20.064</v>
-      </c>
-      <c r="E65" s="3">
-        <v>3.2422456479857191E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>45</v>
-      </c>
-      <c r="D66" s="2">
-        <v>19.960899999999999</v>
-      </c>
-      <c r="E66" s="3">
-        <v>2.4541286215522252E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C67" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="2">
-        <v>65</v>
-      </c>
-      <c r="E67" s="3">
-        <v>4.0178325998604784E-7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
-        <v>59</v>
-      </c>
-      <c r="D68" s="2">
-        <v>11.029199999999999</v>
-      </c>
-      <c r="E68" s="3">
-        <v>0.36358608397346781</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
-        <v>57</v>
-      </c>
-      <c r="C69" t="s">
-        <v>37</v>
-      </c>
-      <c r="D69" s="2">
-        <v>10</v>
-      </c>
-      <c r="E69" s="3">
-        <v>1.236256184572455E-7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
-        <v>60</v>
-      </c>
-      <c r="D70" s="2">
-        <v>10</v>
-      </c>
-      <c r="E70" s="3">
-        <v>1.236256184572455E-7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
-        <v>55</v>
-      </c>
-      <c r="C71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D71" s="2">
-        <v>1.9575</v>
-      </c>
-      <c r="E71" s="3">
-        <v>1.8574131045108848E-4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C72" t="s">
-        <v>29</v>
-      </c>
-      <c r="D72" s="2">
-        <v>6.9623999999999997</v>
-      </c>
-      <c r="E72" s="3">
-        <v>5.4284219228127872E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C73" t="s">
-        <v>30</v>
-      </c>
-      <c r="D73" s="2">
-        <v>6.9691000000000001</v>
-      </c>
-      <c r="E73" s="3">
-        <v>4.0855806750312335E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C74" t="s">
-        <v>31</v>
-      </c>
-      <c r="D74" s="2">
-        <v>13.062799999999999</v>
-      </c>
-      <c r="E74" s="3">
-        <v>1.430153077073168E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C75" t="s">
-        <v>36</v>
-      </c>
-      <c r="D75" s="2">
-        <v>14.9907</v>
-      </c>
-      <c r="E75" s="3">
-        <v>5.1439321771066049E-3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C76" t="s">
-        <v>34</v>
-      </c>
-      <c r="D76" s="2">
-        <v>12.0143</v>
-      </c>
-      <c r="E76" s="3">
-        <v>2.5299883916780525E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C77" t="s">
-        <v>28</v>
-      </c>
-      <c r="D77" s="2">
-        <v>19.044699999999999</v>
-      </c>
-      <c r="E77" s="3">
-        <v>3.6860770714495375E-3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C78" t="s">
-        <v>38</v>
-      </c>
-      <c r="D78" s="2">
-        <v>15.0275</v>
-      </c>
-      <c r="E78" s="3">
-        <v>3.3480463066457064E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
-        <v>58</v>
-      </c>
-      <c r="D79" s="2">
-        <v>8.9879999999999995</v>
-      </c>
-      <c r="E79" s="3">
-        <v>0.17723765429141672</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>46</v>
-      </c>
-      <c r="D80" s="2">
-        <v>10.2652</v>
-      </c>
-      <c r="E80" s="3">
-        <v>0.54082386189050302</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>19</v>
-      </c>
-      <c r="B81" t="s">
-        <v>56</v>
-      </c>
-      <c r="C81" t="s">
-        <v>30</v>
-      </c>
-      <c r="D81" s="2">
-        <v>5.9424999999999999</v>
-      </c>
-      <c r="E81" s="3">
-        <v>1.7462242232704384E-3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C82" t="s">
-        <v>34</v>
-      </c>
-      <c r="D82" s="2">
-        <v>7.9743000000000004</v>
-      </c>
-      <c r="E82" s="3">
-        <v>1.5253670558965692E-3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
-        <v>59</v>
-      </c>
-      <c r="D83" s="2">
-        <v>6.7435999999999998</v>
-      </c>
-      <c r="E83" s="3">
-        <v>3.2715912791670076E-3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>47</v>
-      </c>
-      <c r="D84" s="2">
-        <v>6.7435999999999998</v>
-      </c>
-      <c r="E84" s="3">
-        <v>3.2715912791670076E-3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>20</v>
-      </c>
-      <c r="B85" t="s">
-        <v>56</v>
-      </c>
-      <c r="C85" t="s">
-        <v>28</v>
-      </c>
-      <c r="D85" s="2">
-        <v>2.3332999999999999</v>
-      </c>
-      <c r="E85" s="3">
-        <v>4.3268966460035926E-8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
-        <v>59</v>
-      </c>
-      <c r="D86" s="2">
-        <v>2.3332999999999999</v>
-      </c>
-      <c r="E86" s="3">
-        <v>4.3268966460035926E-8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>48</v>
-      </c>
-      <c r="D87" s="2">
-        <v>2.3332999999999999</v>
-      </c>
-      <c r="E87" s="3">
-        <v>4.3268966460035926E-8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>21</v>
-      </c>
-      <c r="B88" t="s">
-        <v>56</v>
-      </c>
-      <c r="C88" t="s">
-        <v>26</v>
-      </c>
-      <c r="D88" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="E88" s="3">
-        <v>3.0906404614311375E-8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C89" t="s">
-        <v>29</v>
-      </c>
-      <c r="D89" s="2">
-        <v>3.8235000000000001</v>
-      </c>
-      <c r="E89" s="3">
-        <v>4.0178325998604784E-7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C90" t="s">
-        <v>30</v>
-      </c>
-      <c r="D90" s="2">
-        <v>3.2303000000000002</v>
-      </c>
-      <c r="E90" s="3">
-        <v>3.5542365306458079E-6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C91" t="s">
-        <v>34</v>
-      </c>
-      <c r="D91" s="2">
-        <v>5.1802999999999999</v>
-      </c>
-      <c r="E91" s="3">
-        <v>1.9532847716244788E-6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C92" t="s">
-        <v>28</v>
-      </c>
-      <c r="D92" s="2">
-        <v>0.58330000000000004</v>
-      </c>
-      <c r="E92" s="3">
-        <v>4.3268966460035926E-8</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C93" t="s">
-        <v>38</v>
-      </c>
-      <c r="D93" s="2">
-        <v>6.4972000000000003</v>
-      </c>
-      <c r="E93" s="3">
-        <v>3.051805945905163E-2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B94" t="s">
-        <v>59</v>
-      </c>
-      <c r="D94" s="2">
-        <v>6.4961000000000002</v>
-      </c>
-      <c r="E94" s="3">
-        <v>3.052404293898496E-2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B95" t="s">
-        <v>57</v>
-      </c>
-      <c r="C95" t="s">
-        <v>34</v>
-      </c>
-      <c r="D95" s="2">
-        <v>8.4</v>
-      </c>
-      <c r="E95" s="3">
-        <v>2.5961379876021556E-7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B96" t="s">
-        <v>60</v>
-      </c>
-      <c r="D96" s="2">
-        <v>8.4</v>
-      </c>
-      <c r="E96" s="3">
-        <v>2.5961379876021556E-7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B97" t="s">
-        <v>55</v>
-      </c>
-      <c r="C97" t="s">
-        <v>25</v>
-      </c>
-      <c r="D97" s="2">
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="E97" s="3">
-        <v>4.1229143755491375E-6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C98" t="s">
-        <v>30</v>
-      </c>
-      <c r="D98" s="2">
-        <v>6.4927000000000001</v>
-      </c>
-      <c r="E98" s="3">
-        <v>2.8369495660512084E-2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C99" t="s">
-        <v>31</v>
-      </c>
-      <c r="D99" s="2">
-        <v>5.6071</v>
-      </c>
-      <c r="E99" s="3">
-        <v>9.7046110488937719E-7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C100" t="s">
-        <v>34</v>
-      </c>
-      <c r="D100" s="2">
-        <v>10.5608</v>
-      </c>
-      <c r="E100" s="3">
-        <v>3.7758657400069423E-2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C101" t="s">
-        <v>28</v>
-      </c>
-      <c r="D101" s="2">
-        <v>16</v>
-      </c>
-      <c r="E101" s="3">
-        <v>3.9560197906318559E-7</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C102" t="s">
-        <v>38</v>
-      </c>
-      <c r="D102" s="2">
-        <v>15.0189</v>
-      </c>
-      <c r="E102" s="3">
-        <v>2.142595153680428E-2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C103" t="s">
-        <v>35</v>
-      </c>
-      <c r="D103" s="2">
-        <v>25</v>
-      </c>
-      <c r="E103" s="3">
-        <v>1.5453202307155687E-7</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B104" t="s">
-        <v>58</v>
-      </c>
-      <c r="D104" s="2">
-        <v>9.3378999999999994</v>
-      </c>
-      <c r="E104" s="3">
-        <v>8.7559748106868368E-2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>49</v>
-      </c>
-      <c r="D105" s="2">
-        <v>8.3892000000000007</v>
-      </c>
-      <c r="E105" s="3">
-        <v>0.11808405065965208</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>22</v>
-      </c>
-      <c r="B106" t="s">
-        <v>56</v>
-      </c>
-      <c r="C106" t="s">
-        <v>34</v>
-      </c>
-      <c r="D106" s="2">
-        <v>3.6667000000000001</v>
-      </c>
-      <c r="E106" s="3">
-        <v>6.7994090151485029E-8</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B107" t="s">
-        <v>59</v>
-      </c>
-      <c r="D107" s="2">
-        <v>3.6667000000000001</v>
-      </c>
-      <c r="E107" s="3">
-        <v>6.7994090151485029E-8</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>50</v>
-      </c>
-      <c r="D108" s="2">
-        <v>3.6667000000000001</v>
-      </c>
-      <c r="E108" s="3">
-        <v>6.7994090151485029E-8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>23</v>
-      </c>
-      <c r="D109" s="2">
-        <v>6.7496</v>
-      </c>
-      <c r="E109" s="3">
+      <c r="J27" s="6">
         <v>1</v>
       </c>
+      <c r="K27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>